<commit_message>
update errata drift and add new information
</commit_message>
<xml_diff>
--- a/errata_drift.xlsx
+++ b/errata_drift.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
-  <fileSharing readOnlyRecommended="0" userName="christian"/>
+  <fileSharing readOnlyRecommended="0" userName="cstankow"/>
   <workbookPr/>
   <bookViews>
     <workbookView activeTab="0" xWindow="240" yWindow="60" windowWidth="0" windowHeight="0" tabRatio="500"/>
@@ -13,17 +13,17 @@
   <calcPr/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1629269222" val="1016" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1629269222" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1629269222" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1629269222"/>
+      <pm:revision xmlns:pm="smNativeData" day="1632926886" val="1034" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1632926886" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1632926886" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1632926886"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="214">
   <si>
     <t>RHEL</t>
   </si>
@@ -578,6 +578,93 @@
   </si>
   <si>
     <t>ALSA-2021:3157</t>
+  </si>
+  <si>
+    <t>RHSA-2021:3253</t>
+  </si>
+  <si>
+    <t>RLSA-2021:3253</t>
+  </si>
+  <si>
+    <t>ALSA-2021:3253</t>
+  </si>
+  <si>
+    <t>RHSA-2021:3436</t>
+  </si>
+  <si>
+    <t>RHSA-2021:3447</t>
+  </si>
+  <si>
+    <t>RLSA-2021:3447</t>
+  </si>
+  <si>
+    <t>ALSA-2021:3447</t>
+  </si>
+  <si>
+    <t>RHSA-2021:3492</t>
+  </si>
+  <si>
+    <t>ALSA-2021:3492</t>
+  </si>
+  <si>
+    <t>RHSA-2021:3497</t>
+  </si>
+  <si>
+    <t>ALSA-2021:3497</t>
+  </si>
+  <si>
+    <t>RHSA-2021:3499</t>
+  </si>
+  <si>
+    <t>ALSA-2021:3499</t>
+  </si>
+  <si>
+    <t>RHSA-2021:3548</t>
+  </si>
+  <si>
+    <t>ALSA-2021:3548</t>
+  </si>
+  <si>
+    <t>RHSA-2021:3572</t>
+  </si>
+  <si>
+    <t>ALSA-2021:3572</t>
+  </si>
+  <si>
+    <t>RHSA-2021:3576</t>
+  </si>
+  <si>
+    <t>ALSA-2021:3576</t>
+  </si>
+  <si>
+    <t>RHSA-2021:3582</t>
+  </si>
+  <si>
+    <t>ALSA-2021:3582</t>
+  </si>
+  <si>
+    <t>RHSA-2021:3585</t>
+  </si>
+  <si>
+    <t>ALSA-2021:3585</t>
+  </si>
+  <si>
+    <t>RHSA-2021:3590</t>
+  </si>
+  <si>
+    <t>ALSA-2021:3590</t>
+  </si>
+  <si>
+    <t>RHSA-2021:3623</t>
+  </si>
+  <si>
+    <t>ALSA-2021:3623</t>
+  </si>
+  <si>
+    <t>RHSA-2021:3666</t>
+  </si>
+  <si>
+    <t>ALSA-2021:3666</t>
   </si>
 </sst>
 </file>
@@ -596,7 +683,7 @@
     <numFmt numFmtId="14" formatCode="DD/MM/YYYY"/>
     <numFmt numFmtId="3" formatCode="#,##0"/>
   </numFmts>
-  <fonts count="170">
+  <fonts count="199">
     <font>
       <name val="Arial"/>
       <family val="2"/>
@@ -604,7 +691,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -619,7 +706,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" ulstyle="none" kern="1">
             <pm:latin face="Basic Sans" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -634,23 +721,23 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" ulstyle="none" kern="1">
-            <pm:latin face="Arial" sz="200" lang="default"/>
-            <pm:cs face="Basic Roman" sz="200" lang="default"/>
-            <pm:ea face="Basic Roman" sz="200" lang="default"/>
-          </pm:charSpec>
-        </ext>
-      </extLst>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <family val="2"/>
-      <color rgb="FF0000FF"/>
-      <sz val="10"/>
-      <u val="single"/>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" ulstyle="none" kern="1">
+            <pm:latin face="Arial" sz="200" lang="default"/>
+            <pm:cs face="Basic Roman" sz="200" lang="default"/>
+            <pm:ea face="Basic Roman" sz="200" lang="default"/>
+          </pm:charSpec>
+        </ext>
+      </extLst>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="2"/>
+      <color rgb="FF0000FF"/>
+      <sz val="10"/>
+      <u val="single"/>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -667,23 +754,23 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
-            <pm:latin face="Arial" sz="200" lang="default"/>
-            <pm:cs face="Basic Roman" sz="200" lang="default"/>
-            <pm:ea face="Basic Roman" sz="200" lang="default"/>
-          </pm:charSpec>
-        </ext>
-      </extLst>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <family val="2"/>
-      <color rgb="FF0000FF"/>
-      <sz val="10"/>
-      <u val="single"/>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
+            <pm:latin face="Arial" sz="200" lang="default"/>
+            <pm:cs face="Basic Roman" sz="200" lang="default"/>
+            <pm:ea face="Basic Roman" sz="200" lang="default"/>
+          </pm:charSpec>
+        </ext>
+      </extLst>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="2"/>
+      <color rgb="FF0000FF"/>
+      <sz val="10"/>
+      <u val="single"/>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -700,7 +787,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -717,7 +804,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -734,7 +821,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -751,7 +838,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -768,7 +855,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -785,7 +872,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -802,7 +889,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -819,7 +906,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -836,7 +923,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -853,7 +940,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -870,7 +957,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -887,7 +974,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -904,7 +991,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -921,7 +1008,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -938,7 +1025,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -955,7 +1042,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -972,7 +1059,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default" weight="bold"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -988,7 +1075,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -1005,7 +1092,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -1022,7 +1109,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -1039,7 +1126,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -1056,7 +1143,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -1073,7 +1160,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -1090,7 +1177,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -1107,7 +1194,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -1124,7 +1211,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -1141,7 +1228,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -1158,7 +1245,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -1175,7 +1262,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -1192,7 +1279,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -1209,7 +1296,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -1226,7 +1313,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -1243,7 +1330,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -1260,7 +1347,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -1277,7 +1364,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -1294,7 +1381,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -1311,7 +1398,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -1328,7 +1415,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -1345,7 +1432,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -1362,7 +1449,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -1379,7 +1466,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -1396,7 +1483,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -1413,7 +1500,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -1430,7 +1517,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -1447,7 +1534,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -1464,7 +1551,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -1481,7 +1568,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -1498,7 +1585,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -1515,7 +1602,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -1532,7 +1619,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -1549,7 +1636,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -1566,7 +1653,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -1583,7 +1670,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -1600,7 +1687,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -1617,7 +1704,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -1634,7 +1721,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -1651,7 +1738,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -1668,7 +1755,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -1685,7 +1772,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -1702,7 +1789,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -1719,7 +1806,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -1736,7 +1823,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -1753,7 +1840,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -1770,7 +1857,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -1787,7 +1874,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -1804,7 +1891,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -1821,7 +1908,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -1838,7 +1925,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -1855,7 +1942,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -1872,7 +1959,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -1889,7 +1976,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -1906,7 +1993,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -1923,7 +2010,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -1940,7 +2027,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -1957,7 +2044,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -1974,7 +2061,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -1991,7 +2078,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -2008,7 +2095,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -2025,7 +2112,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -2042,7 +2129,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -2059,7 +2146,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -2076,7 +2163,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -2093,7 +2180,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -2110,7 +2197,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -2127,7 +2214,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -2144,7 +2231,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -2161,7 +2248,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -2178,7 +2265,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -2195,7 +2282,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -2212,7 +2299,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -2229,7 +2316,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -2246,7 +2333,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -2263,7 +2350,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -2280,7 +2367,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -2297,7 +2384,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -2314,7 +2401,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -2331,7 +2418,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -2348,7 +2435,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -2365,7 +2452,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -2382,7 +2469,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -2399,7 +2486,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -2416,7 +2503,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -2433,7 +2520,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -2450,7 +2537,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -2467,7 +2554,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -2484,7 +2571,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -2501,7 +2588,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -2518,7 +2605,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -2535,7 +2622,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -2552,7 +2639,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -2569,7 +2656,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -2586,7 +2673,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -2603,7 +2690,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -2620,7 +2707,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -2637,7 +2724,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -2654,7 +2741,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -2671,7 +2758,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -2688,7 +2775,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -2705,7 +2792,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -2722,7 +2809,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -2739,7 +2826,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -2756,7 +2843,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -2773,7 +2860,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -2790,7 +2877,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -2807,7 +2894,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -2824,7 +2911,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -2841,7 +2928,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -2858,7 +2945,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -2875,7 +2962,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -2892,7 +2979,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -2909,7 +2996,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -2926,7 +3013,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -2943,7 +3030,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -2960,7 +3047,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -2977,7 +3064,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -2994,7 +3081,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -3011,7 +3098,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -3028,7 +3115,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -3045,7 +3132,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -3062,7 +3149,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -3079,7 +3166,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -3096,7 +3183,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -3113,7 +3200,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -3130,7 +3217,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -3147,7 +3234,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -3164,7 +3251,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -3181,7 +3268,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -3198,7 +3285,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -3215,7 +3302,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -3232,7 +3319,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -3249,7 +3336,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -3266,7 +3353,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -3283,7 +3370,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -3300,7 +3387,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -3317,7 +3404,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -3334,7 +3421,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -3351,7 +3438,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -3368,7 +3455,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -3385,7 +3472,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -3402,7 +3489,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -3419,7 +3506,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -3436,7 +3523,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -3453,7 +3540,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -3470,7 +3557,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1629269222" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -3479,8 +3566,501 @@
         </ext>
       </extLst>
     </font>
+    <font>
+      <name val="Arial"/>
+      <family val="2"/>
+      <color rgb="FF0000FF"/>
+      <sz val="10"/>
+      <u val="single"/>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
+            <pm:latin face="Arial" sz="200" lang="default"/>
+            <pm:cs face="Basic Roman" sz="200" lang="default"/>
+            <pm:ea face="Basic Roman" sz="200" lang="default"/>
+            <hyperlink type="6" url="https://access.redhat.com/errata/RHSA-2021:3253" location="" text=""/>
+          </pm:charSpec>
+        </ext>
+      </extLst>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="2"/>
+      <color rgb="FF0000FF"/>
+      <sz val="10"/>
+      <u val="single"/>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
+            <pm:latin face="Arial" sz="200" lang="default"/>
+            <pm:cs face="Basic Roman" sz="200" lang="default"/>
+            <pm:ea face="Basic Roman" sz="200" lang="default"/>
+            <hyperlink type="6" url="https://access.redhat.com/errata/RHSA-2021:3436" location="" text=""/>
+          </pm:charSpec>
+        </ext>
+      </extLst>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="2"/>
+      <color rgb="FF0000FF"/>
+      <sz val="10"/>
+      <u val="single"/>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
+            <pm:latin face="Arial" sz="200" lang="default"/>
+            <pm:cs face="Basic Roman" sz="200" lang="default"/>
+            <pm:ea face="Basic Roman" sz="200" lang="default"/>
+            <hyperlink type="6" url="https://access.redhat.com/errata/RHSA-2021:3447" location="" text=""/>
+          </pm:charSpec>
+        </ext>
+      </extLst>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="2"/>
+      <color rgb="FF0000FF"/>
+      <sz val="10"/>
+      <u val="single"/>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
+            <pm:latin face="Arial" sz="200" lang="default"/>
+            <pm:cs face="Basic Roman" sz="200" lang="default"/>
+            <pm:ea face="Basic Roman" sz="200" lang="default"/>
+            <hyperlink type="6" url="https://access.redhat.com/errata/RHSA-2021:3492" location="" text=""/>
+          </pm:charSpec>
+        </ext>
+      </extLst>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="2"/>
+      <color rgb="FF0000FF"/>
+      <sz val="10"/>
+      <u val="single"/>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
+            <pm:latin face="Arial" sz="200" lang="default"/>
+            <pm:cs face="Basic Roman" sz="200" lang="default"/>
+            <pm:ea face="Basic Roman" sz="200" lang="default"/>
+            <hyperlink type="6" url="https://access.redhat.com/errata/RHSA-2021:3497" location="" text=""/>
+          </pm:charSpec>
+        </ext>
+      </extLst>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="2"/>
+      <color rgb="FF0000FF"/>
+      <sz val="10"/>
+      <u val="single"/>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
+            <pm:latin face="Arial" sz="200" lang="default"/>
+            <pm:cs face="Basic Roman" sz="200" lang="default"/>
+            <pm:ea face="Basic Roman" sz="200" lang="default"/>
+            <hyperlink type="6" url="https://access.redhat.com/errata/RHSA-2021:3499" location="" text=""/>
+          </pm:charSpec>
+        </ext>
+      </extLst>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="2"/>
+      <color rgb="FF0000FF"/>
+      <sz val="10"/>
+      <u val="single"/>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
+            <pm:latin face="Arial" sz="200" lang="default"/>
+            <pm:cs face="Basic Roman" sz="200" lang="default"/>
+            <pm:ea face="Basic Roman" sz="200" lang="default"/>
+            <hyperlink type="6" url="https://access.redhat.com/errata/RHSA-2021:3548" location="" text=""/>
+          </pm:charSpec>
+        </ext>
+      </extLst>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="2"/>
+      <color rgb="FF0000FF"/>
+      <sz val="10"/>
+      <u val="single"/>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
+            <pm:latin face="Arial" sz="200" lang="default"/>
+            <pm:cs face="Basic Roman" sz="200" lang="default"/>
+            <pm:ea face="Basic Roman" sz="200" lang="default"/>
+            <hyperlink type="6" url="https://access.redhat.com/errata/RHSA-2021:3572" location="" text=""/>
+          </pm:charSpec>
+        </ext>
+      </extLst>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="2"/>
+      <color rgb="FF0000FF"/>
+      <sz val="10"/>
+      <u val="single"/>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
+            <pm:latin face="Arial" sz="200" lang="default"/>
+            <pm:cs face="Basic Roman" sz="200" lang="default"/>
+            <pm:ea face="Basic Roman" sz="200" lang="default"/>
+            <hyperlink type="6" url="https://access.redhat.com/errata/RHSA-2021:3576" location="" text=""/>
+          </pm:charSpec>
+        </ext>
+      </extLst>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="2"/>
+      <color rgb="FF0000FF"/>
+      <sz val="10"/>
+      <u val="single"/>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
+            <pm:latin face="Arial" sz="200" lang="default"/>
+            <pm:cs face="Basic Roman" sz="200" lang="default"/>
+            <pm:ea face="Basic Roman" sz="200" lang="default"/>
+            <hyperlink type="6" url="https://access.redhat.com/errata/RHSA-2021:3582" location="" text=""/>
+          </pm:charSpec>
+        </ext>
+      </extLst>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="2"/>
+      <color rgb="FF0000FF"/>
+      <sz val="10"/>
+      <u val="single"/>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
+            <pm:latin face="Arial" sz="200" lang="default"/>
+            <pm:cs face="Basic Roman" sz="200" lang="default"/>
+            <pm:ea face="Basic Roman" sz="200" lang="default"/>
+            <hyperlink type="6" url="https://access.redhat.com/errata/RHSA-2021:3585" location="" text=""/>
+          </pm:charSpec>
+        </ext>
+      </extLst>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="2"/>
+      <color rgb="FF0000FF"/>
+      <sz val="10"/>
+      <u val="single"/>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
+            <pm:latin face="Arial" sz="200" lang="default"/>
+            <pm:cs face="Basic Roman" sz="200" lang="default"/>
+            <pm:ea face="Basic Roman" sz="200" lang="default"/>
+            <hyperlink type="6" url="https://access.redhat.com/errata/RHSA-2021:3590" location="" text=""/>
+          </pm:charSpec>
+        </ext>
+      </extLst>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="2"/>
+      <color rgb="FF0000FF"/>
+      <sz val="10"/>
+      <u val="single"/>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
+            <pm:latin face="Arial" sz="200" lang="default"/>
+            <pm:cs face="Basic Roman" sz="200" lang="default"/>
+            <pm:ea face="Basic Roman" sz="200" lang="default"/>
+            <hyperlink type="6" url="https://access.redhat.com/errata/RHSA-2021:3623" location="" text=""/>
+          </pm:charSpec>
+        </ext>
+      </extLst>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="2"/>
+      <color rgb="FF0000FF"/>
+      <sz val="10"/>
+      <u val="single"/>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
+            <pm:latin face="Arial" sz="200" lang="default"/>
+            <pm:cs face="Basic Roman" sz="200" lang="default"/>
+            <pm:ea face="Basic Roman" sz="200" lang="default"/>
+            <hyperlink type="6" url="https://access.redhat.com/errata/RHSA-2021:3666" location="" text=""/>
+          </pm:charSpec>
+        </ext>
+      </extLst>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="2"/>
+      <color rgb="FF0000FF"/>
+      <sz val="10"/>
+      <u val="single"/>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
+            <pm:latin face="Arial" sz="200" lang="default"/>
+            <pm:cs face="Basic Roman" sz="200" lang="default"/>
+            <pm:ea face="Basic Roman" sz="200" lang="default"/>
+            <hyperlink type="6" url="https://errata.almalinux.org/8/ALSA-2021-3253.html" location="" text=""/>
+          </pm:charSpec>
+        </ext>
+      </extLst>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="2"/>
+      <color rgb="FF0000FF"/>
+      <sz val="10"/>
+      <u val="single"/>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
+            <pm:latin face="Arial" sz="200" lang="default"/>
+            <pm:cs face="Basic Roman" sz="200" lang="default"/>
+            <pm:ea face="Basic Roman" sz="200" lang="default"/>
+            <hyperlink type="6" url="https://errata.almalinux.org/8/ALSA-2021-3447.html" location="" text=""/>
+          </pm:charSpec>
+        </ext>
+      </extLst>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="2"/>
+      <color rgb="FF0000FF"/>
+      <sz val="10"/>
+      <u val="single"/>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
+            <pm:latin face="Arial" sz="200" lang="default"/>
+            <pm:cs face="Basic Roman" sz="200" lang="default"/>
+            <pm:ea face="Basic Roman" sz="200" lang="default"/>
+            <hyperlink type="6" url="https://errata.almalinux.org/8/ALSA-2021-3492.html" location="" text=""/>
+          </pm:charSpec>
+        </ext>
+      </extLst>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="2"/>
+      <color rgb="FF0000FF"/>
+      <sz val="10"/>
+      <u val="single"/>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
+            <pm:latin face="Arial" sz="200" lang="default"/>
+            <pm:cs face="Basic Roman" sz="200" lang="default"/>
+            <pm:ea face="Basic Roman" sz="200" lang="default"/>
+            <hyperlink type="6" url="https://errata.almalinux.org/8/ALSA-2021-3497.html" location="" text=""/>
+          </pm:charSpec>
+        </ext>
+      </extLst>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="2"/>
+      <color rgb="FF0000FF"/>
+      <sz val="10"/>
+      <u val="single"/>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
+            <pm:latin face="Arial" sz="200" lang="default"/>
+            <pm:cs face="Basic Roman" sz="200" lang="default"/>
+            <pm:ea face="Basic Roman" sz="200" lang="default"/>
+            <hyperlink type="6" url="https://errata.almalinux.org/8/ALSA-2021-3499.html" location="" text=""/>
+          </pm:charSpec>
+        </ext>
+      </extLst>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="2"/>
+      <color rgb="FF0000FF"/>
+      <sz val="10"/>
+      <u val="single"/>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
+            <pm:latin face="Arial" sz="200" lang="default"/>
+            <pm:cs face="Basic Roman" sz="200" lang="default"/>
+            <pm:ea face="Basic Roman" sz="200" lang="default"/>
+            <hyperlink type="6" url="https://errata.almalinux.org/8/ALSA-2021-3548.html" location="" text=""/>
+          </pm:charSpec>
+        </ext>
+      </extLst>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="2"/>
+      <color rgb="FF0000FF"/>
+      <sz val="10"/>
+      <u val="single"/>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
+            <pm:latin face="Arial" sz="200" lang="default"/>
+            <pm:cs face="Basic Roman" sz="200" lang="default"/>
+            <pm:ea face="Basic Roman" sz="200" lang="default"/>
+            <hyperlink type="6" url="https://errata.almalinux.org/8/ALSA-2021-3572.html" location="" text=""/>
+          </pm:charSpec>
+        </ext>
+      </extLst>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="2"/>
+      <color rgb="FF0000FF"/>
+      <sz val="10"/>
+      <u val="single"/>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
+            <pm:latin face="Arial" sz="200" lang="default"/>
+            <pm:cs face="Basic Roman" sz="200" lang="default"/>
+            <pm:ea face="Basic Roman" sz="200" lang="default"/>
+            <hyperlink type="6" url="https://errata.almalinux.org/8/ALSA-2021-3576.html" location="" text=""/>
+          </pm:charSpec>
+        </ext>
+      </extLst>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="2"/>
+      <color rgb="FF0000FF"/>
+      <sz val="10"/>
+      <u val="single"/>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
+            <pm:latin face="Arial" sz="200" lang="default"/>
+            <pm:cs face="Basic Roman" sz="200" lang="default"/>
+            <pm:ea face="Basic Roman" sz="200" lang="default"/>
+            <hyperlink type="6" url="https://errata.almalinux.org/8/ALSA-2021-3582.html" location="" text=""/>
+          </pm:charSpec>
+        </ext>
+      </extLst>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="2"/>
+      <color rgb="FF0000FF"/>
+      <sz val="10"/>
+      <u val="single"/>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
+            <pm:latin face="Arial" sz="200" lang="default"/>
+            <pm:cs face="Basic Roman" sz="200" lang="default"/>
+            <pm:ea face="Basic Roman" sz="200" lang="default"/>
+            <hyperlink type="6" url="https://errata.almalinux.org/8/ALSA-2021-3585.html" location="" text=""/>
+          </pm:charSpec>
+        </ext>
+      </extLst>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="2"/>
+      <color rgb="FF0000FF"/>
+      <sz val="10"/>
+      <u val="single"/>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
+            <pm:latin face="Arial" sz="200" lang="default"/>
+            <pm:cs face="Basic Roman" sz="200" lang="default"/>
+            <pm:ea face="Basic Roman" sz="200" lang="default"/>
+            <hyperlink type="6" url="https://errata.almalinux.org/8/ALSA-2021-3590.html" location="" text=""/>
+          </pm:charSpec>
+        </ext>
+      </extLst>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="2"/>
+      <color rgb="FF0000FF"/>
+      <sz val="10"/>
+      <u val="single"/>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
+            <pm:latin face="Arial" sz="200" lang="default"/>
+            <pm:cs face="Basic Roman" sz="200" lang="default"/>
+            <pm:ea face="Basic Roman" sz="200" lang="default"/>
+            <hyperlink type="6" url="https://errata.almalinux.org/8/ALSA-2021-3623.html" location="" text=""/>
+          </pm:charSpec>
+        </ext>
+      </extLst>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="2"/>
+      <color rgb="FF0000FF"/>
+      <sz val="10"/>
+      <u val="single"/>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
+            <pm:latin face="Arial" sz="200" lang="default"/>
+            <pm:cs face="Basic Roman" sz="200" lang="default"/>
+            <pm:ea face="Basic Roman" sz="200" lang="default"/>
+            <hyperlink type="6" url="https://errata.almalinux.org/8/ALSA-2021-3666.html" location="" text=""/>
+          </pm:charSpec>
+        </ext>
+      </extLst>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="2"/>
+      <color rgb="FF0000FF"/>
+      <sz val="10"/>
+      <u val="single"/>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
+            <pm:latin face="Arial" sz="200" lang="default"/>
+            <pm:cs face="Basic Roman" sz="200" lang="default"/>
+            <pm:ea face="Basic Roman" sz="200" lang="default"/>
+            <hyperlink type="6" url="https://errata.rockylinux.org/RLSA-2021:3253" location="" text=""/>
+          </pm:charSpec>
+        </ext>
+      </extLst>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="2"/>
+      <color rgb="FF0000FF"/>
+      <sz val="10"/>
+      <u val="single"/>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:charSpec xmlns:pm="smNativeData" id="1632926886" fgClr="0000FF" ulstyle="single" kern="1">
+            <pm:latin face="Arial" sz="200" lang="default"/>
+            <pm:cs face="Basic Roman" sz="200" lang="default"/>
+            <pm:ea face="Basic Roman" sz="200" lang="default"/>
+            <hyperlink type="6" url="https://errata.rockylinux.org/RLSA-2021:3447" location="" text=""/>
+          </pm:charSpec>
+        </ext>
+      </extLst>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3517,13 +4097,16 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1629269222" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1632926886" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none"/>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left style="none">
         <color rgb="FF000000"/>
@@ -3539,7 +4122,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1629269222"/>
+          <pm:border xmlns:pm="smNativeData" id="1632926886"/>
         </ext>
       </extLst>
     </border>
@@ -3558,7 +4141,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1629269222">
+          <pm:border xmlns:pm="smNativeData" id="1632926886">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
@@ -3582,7 +4165,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1629269222">
+          <pm:border xmlns:pm="smNativeData" id="1632926886">
             <pm:line position="top" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
           </pm:border>
@@ -3604,7 +4187,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1629269222">
+          <pm:border xmlns:pm="smNativeData" id="1632926886">
             <pm:line position="top" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
           </pm:border>
         </ext>
@@ -3625,7 +4208,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1629269222">
+          <pm:border xmlns:pm="smNativeData" id="1632926886">
             <pm:line position="top" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
             <pm:line position="right" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
           </pm:border>
@@ -3647,7 +4230,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1629269222">
+          <pm:border xmlns:pm="smNativeData" id="1632926886">
             <pm:line position="bottom" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
           </pm:border>
@@ -3669,7 +4252,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1629269222">
+          <pm:border xmlns:pm="smNativeData" id="1632926886">
             <pm:line position="bottom" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
           </pm:border>
         </ext>
@@ -3690,7 +4273,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1629269222">
+          <pm:border xmlns:pm="smNativeData" id="1632926886">
             <pm:line position="bottom" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
             <pm:line position="right" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
           </pm:border>
@@ -3712,7 +4295,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1629269222">
+          <pm:border xmlns:pm="smNativeData" id="1632926886">
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="right" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
@@ -3735,7 +4318,30 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1629269222"/>
+          <pm:border xmlns:pm="smNativeData" id="1632926886"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1632926886">
+            <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
+            <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
+            <pm:line position="right" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
+          </pm:border>
         </ext>
       </extLst>
     </border>
@@ -3744,200 +4350,239 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="183">
+  <cellXfs count="222">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="111" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="112" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="113" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="114" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="115" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="116" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="117" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="118" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="48" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="119" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="49" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="120" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="50" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="121" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="51" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="122" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="123" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="124" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="54" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="125" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="55" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="126" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="56" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="127" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="57" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="128" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="58" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="129" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="59" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="130" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="60" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="131" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="132" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="61" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="133" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="62" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="134" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="63" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="135" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="64" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="136" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="137" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="65" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="138" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="66" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="139" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="111" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="112" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="113" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="114" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="115" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="116" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="117" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="118" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="119" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="120" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="121" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="122" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="123" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="124" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="54" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="125" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="55" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="126" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="56" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="127" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="57" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="128" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="58" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="129" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="59" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="130" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="60" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="131" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="132" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="61" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="133" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="62" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="134" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="63" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="135" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="64" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="136" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="137" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="65" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="138" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="66" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="139" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="67" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="140" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="67" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="140" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="68" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="141" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="69" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="142" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="70" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="143" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="144" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="71" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="145" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="72" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="146" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="73" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="147" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="68" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="141" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="69" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="142" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="70" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="143" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="144" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="71" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="145" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="72" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="146" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="73" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="147" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="74" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="148" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="75" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="149" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="76" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="150" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="77" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="151" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="78" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="152" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="79" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="97" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="153" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="80" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="98" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="154" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="81" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="99" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="155" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="82" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="100" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="156" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="83" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="157" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="84" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="101" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="158" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="85" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="102" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="159" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="86" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="160" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="87" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="161" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="88" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="162" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="89" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="103" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="163" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="90" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="104" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="164" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="91" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="105" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="165" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="92" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="106" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="166" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="74" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="148" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="75" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="149" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="76" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="150" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="77" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="151" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="78" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="152" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="79" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="97" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="153" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="80" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="98" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="154" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="81" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="99" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="155" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="82" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="100" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="156" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="83" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="157" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="84" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="101" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="158" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="85" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="102" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="159" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="86" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="160" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="87" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="161" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="88" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="162" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="89" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="103" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="163" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="90" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="104" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="164" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="91" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="105" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="165" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="92" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="106" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="166" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="93" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="107" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="94" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="108" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="167" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="95" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="109" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="168" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="96" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="110" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="169" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="93" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="107" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="94" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="108" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="167" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="95" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="109" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="168" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="170" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="197" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="184" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="171" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="172" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="198" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="185" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="173" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="186" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="174" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="187" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="175" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="188" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="176" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="189" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="177" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="190" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="178" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="191" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="179" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="192" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="180" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="193" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="181" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="194" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="182" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="195" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="183" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="196" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="96" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="110" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="169" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
@@ -3946,7 +4591,7 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1629269222" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1632926886" count="1">
         <pm:charStyle name="Normal" fontId="0"/>
       </pm:charStyles>
     </ext>
@@ -3971,11 +4616,27 @@
           <c:tx>
             <c:v>Rocky</c:v>
           </c:tx>
+          <c:dLbls>
+            <c:numFmt formatCode="General" sourceLinked="1"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Tabelle1!$C$4:$C$63</c:f>
+              <c:f>Tabelle1!$C$4:$C$77</c:f>
               <c:strCache>
-                <c:ptCount val="60"/>
+                <c:ptCount val="74"/>
                 <c:pt idx="0">
                   <c:v>RHSA-2021:2168</c:v>
                 </c:pt>
@@ -4155,16 +4816,58 @@
                 </c:pt>
                 <c:pt idx="59">
                   <c:v>RHSA-2021:3157</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>RHSA-2021:3253</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>RHSA-2021:3436</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>RHSA-2021:3447</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>RHSA-2021:3492</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>RHSA-2021:3497</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>RHSA-2021:3499</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>RHSA-2021:3548</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>RHSA-2021:3572</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>RHSA-2021:3576</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>RHSA-2021:3582</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>RHSA-2021:3585</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>RHSA-2021:3590</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>RHSA-2021:3623</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>RHSA-2021:3666</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$J$4:$J$63</c:f>
+              <c:f>Tabelle1!$J$4:$J$77</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="60"/>
+                <c:ptCount val="74"/>
                 <c:pt idx="0">
                   <c:v>51</c:v>
                 </c:pt>
@@ -4344,6 +5047,48 @@
                 </c:pt>
                 <c:pt idx="59">
                   <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="61" formatCode="General">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="63" formatCode="General">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="64" formatCode="General">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="65" formatCode="General">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="66" formatCode="General">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="67" formatCode="General">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="68" formatCode="General">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="69" formatCode="General">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="70" formatCode="General">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="71" formatCode="General">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="72" formatCode="General">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="73" formatCode="General">
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4353,28 +5098,28 @@
             <c:ext xmlns:sm="smo" uri="smo">
               <sm:meanLine>
                 <c:spPr>
-                  <a:ln>
+                  <a:ln w="9525">
                     <a:noFill/>
                   </a:ln>
                 </c:spPr>
               </sm:meanLine>
               <sm:minMaxLine>
                 <c:spPr>
-                  <a:ln>
+                  <a:ln w="9525">
                     <a:noFill/>
                   </a:ln>
                 </c:spPr>
               </sm:minMaxLine>
               <sm:stDevLine>
                 <c:spPr>
-                  <a:ln>
+                  <a:ln w="9525">
                     <a:noFill/>
                   </a:ln>
                 </c:spPr>
               </sm:stDevLine>
               <sm:trendLine>
                 <c:spPr>
-                  <a:ln>
+                  <a:ln w="9525">
                     <a:noFill/>
                   </a:ln>
                 </c:spPr>
@@ -4390,9 +5135,9 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>Tabelle1!$C$4:$C$63</c:f>
+              <c:f>Tabelle1!$C$4:$C$77</c:f>
               <c:strCache>
-                <c:ptCount val="60"/>
+                <c:ptCount val="74"/>
                 <c:pt idx="0">
                   <c:v>RHSA-2021:2168</c:v>
                 </c:pt>
@@ -4572,16 +5317,58 @@
                 </c:pt>
                 <c:pt idx="59">
                   <c:v>RHSA-2021:3157</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>RHSA-2021:3253</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>RHSA-2021:3436</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>RHSA-2021:3447</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>RHSA-2021:3492</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>RHSA-2021:3497</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>RHSA-2021:3499</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>RHSA-2021:3548</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>RHSA-2021:3572</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>RHSA-2021:3576</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>RHSA-2021:3582</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>RHSA-2021:3585</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>RHSA-2021:3590</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>RHSA-2021:3623</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>RHSA-2021:3666</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$M$4:$M$63</c:f>
+              <c:f>Tabelle1!$M$4:$M$77</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="60"/>
+                <c:ptCount val="74"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -4761,6 +5548,48 @@
                 </c:pt>
                 <c:pt idx="59">
                   <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4770,28 +5599,28 @@
             <c:ext xmlns:sm="smo" uri="smo">
               <sm:meanLine>
                 <c:spPr>
-                  <a:ln>
+                  <a:ln w="9525">
                     <a:noFill/>
                   </a:ln>
                 </c:spPr>
               </sm:meanLine>
               <sm:minMaxLine>
                 <c:spPr>
-                  <a:ln>
+                  <a:ln w="9525">
                     <a:noFill/>
                   </a:ln>
                 </c:spPr>
               </sm:minMaxLine>
               <sm:stDevLine>
                 <c:spPr>
-                  <a:ln>
+                  <a:ln w="9525">
                     <a:noFill/>
                   </a:ln>
                 </c:spPr>
               </sm:stDevLine>
               <sm:trendLine>
                 <c:spPr>
-                  <a:ln>
+                  <a:ln w="9525">
                     <a:noFill/>
                   </a:ln>
                 </c:spPr>
@@ -4834,12 +5663,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr lang="de-de" sz="1800" b="0" i="0" u="none" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Basic Sans" charset="0"/>
-              </a:defRPr>
+              <a:defRPr/>
             </a:pPr>
           </a:p>
         </c:txPr>
@@ -4859,20 +5683,6 @@
         <c:majorTickMark val="cross"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr lang="de-de" sz="1800" b="0" i="0" u="none" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Basic Sans" charset="0"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
         <c:crossAx val="10"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
@@ -4882,17 +5692,17 @@
       <c:legendPos val="r"/>
       <c:layout/>
       <c:overlay val="0"/>
+      <c:spPr>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
       <c:txPr>
         <a:bodyPr anchor="t"/>
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr lang="de-de" sz="1800" b="0" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Basic Sans" charset="0"/>
-            </a:defRPr>
+            <a:defRPr/>
           </a:pPr>
         </a:p>
       </c:txPr>
@@ -4906,18 +5716,18 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr lang="de-de" sz="1800" b="0" i="0" u="none" strike="noStrike">
+        <a:defRPr lang="de-de" sz="1800" b="0" i="0" u="none" strike="noStrike" kern="100">
           <a:solidFill>
             <a:srgbClr val="000000"/>
           </a:solidFill>
-          <a:latin typeface="Basic Sans"/>
+          <a:latin typeface="Basic Sans" charset="0"/>
         </a:defRPr>
       </a:pPr>
     </a:p>
   </c:txPr>
   <c:extLst>
     <c:ext xmlns:sm="smo" uri="smo">
-      <sm:colorScheme xmlns:sm="smo" id="1629269222" val="7"/>
+      <sm:colorScheme xmlns:sm="smo" id="1632926886" val="7"/>
     </c:ext>
   </c:extLst>
 </c:chartSpace>
@@ -5214,10 +6024,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P63"/>
+  <dimension ref="A1:P108"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="normal" workbookViewId="0">
-      <selection activeCell="P19" sqref="P19"/>
+    <sheetView tabSelected="1" view="normal" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="Q5" sqref="Q5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="9" defaultColWidth="10.000000" defaultRowHeight="12.90"/>
@@ -5236,108 +6046,108 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16">
-      <c r="A1" s="172"/>
-      <c r="B1" s="173"/>
-      <c r="C1" s="174" t="s">
+      <c r="A1" s="169"/>
+      <c r="B1" s="170"/>
+      <c r="C1" s="171" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="174"/>
-      <c r="E1" s="174" t="s">
+      <c r="D1" s="171"/>
+      <c r="E1" s="171" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="174"/>
-      <c r="G1" s="175"/>
-      <c r="H1" s="174" t="s">
+      <c r="F1" s="171"/>
+      <c r="G1" s="172"/>
+      <c r="H1" s="171" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="174"/>
-      <c r="J1" s="175"/>
-      <c r="K1" s="174" t="s">
+      <c r="I1" s="171"/>
+      <c r="J1" s="172"/>
+      <c r="K1" s="171" t="s">
         <v>3</v>
       </c>
-      <c r="L1" s="174"/>
-      <c r="M1" s="175"/>
-      <c r="N1" s="174" t="s">
+      <c r="L1" s="171"/>
+      <c r="M1" s="172"/>
+      <c r="N1" s="171" t="s">
         <v>4</v>
       </c>
-      <c r="O1" s="174"/>
-      <c r="P1" s="176"/>
+      <c r="O1" s="171"/>
+      <c r="P1" s="173"/>
     </row>
     <row r="2" spans="1:16">
-      <c r="A2" s="177" t="s">
+      <c r="A2" s="174" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="178" t="s">
+      <c r="B2" s="175" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="178" t="s">
+      <c r="C2" s="175" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="178" t="s">
+      <c r="D2" s="175" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="178" t="s">
+      <c r="E2" s="175" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="178" t="s">
+      <c r="F2" s="175" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="178" t="s">
+      <c r="G2" s="175" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="178" t="s">
+      <c r="H2" s="175" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="178" t="s">
+      <c r="I2" s="175" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="178" t="s">
+      <c r="J2" s="175" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="178" t="s">
+      <c r="K2" s="175" t="s">
         <v>7</v>
       </c>
-      <c r="L2" s="178" t="s">
+      <c r="L2" s="175" t="s">
         <v>8</v>
       </c>
-      <c r="M2" s="178" t="s">
+      <c r="M2" s="175" t="s">
         <v>9</v>
       </c>
-      <c r="N2" s="178" t="s">
+      <c r="N2" s="175" t="s">
         <v>7</v>
       </c>
-      <c r="O2" s="178" t="s">
+      <c r="O2" s="175" t="s">
         <v>8</v>
       </c>
-      <c r="P2" s="179" t="s">
+      <c r="P2" s="176" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:16">
-      <c r="A3" s="180" t="s">
+      <c r="A3" s="177" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="180" t="s">
+      <c r="B3" s="177" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="181" t="s">
+      <c r="C3" s="178" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="182" t="n">
+      <c r="D3" s="179" t="n">
         <v>44348</v>
       </c>
-      <c r="E3" s="180"/>
-      <c r="F3" s="180"/>
-      <c r="G3" s="180"/>
-      <c r="H3" s="180"/>
-      <c r="I3" s="180"/>
-      <c r="J3" s="180"/>
-      <c r="K3" s="180"/>
-      <c r="L3" s="180"/>
-      <c r="M3" s="180"/>
-      <c r="N3" s="180"/>
-      <c r="O3" s="180"/>
-      <c r="P3" s="180"/>
+      <c r="E3" s="177"/>
+      <c r="F3" s="177"/>
+      <c r="G3" s="177"/>
+      <c r="H3" s="177"/>
+      <c r="I3" s="177"/>
+      <c r="J3" s="177"/>
+      <c r="K3" s="177"/>
+      <c r="L3" s="177"/>
+      <c r="M3" s="177"/>
+      <c r="N3" s="177"/>
+      <c r="O3" s="177"/>
+      <c r="P3" s="177"/>
     </row>
     <row r="4" spans="1:16">
       <c r="A4" s="2" t="s">
@@ -7630,44 +8440,564 @@
       <c r="P62" s="2"/>
     </row>
     <row r="63" spans="1:16">
-      <c r="A63" s="2" t="s">
+      <c r="A63" s="216" t="s">
         <v>10</v>
       </c>
-      <c r="B63" s="2" t="s">
+      <c r="B63" s="216" t="s">
         <v>11</v>
       </c>
-      <c r="C63" s="169" t="s">
+      <c r="C63" s="217" t="s">
         <v>182</v>
       </c>
-      <c r="D63" s="4" t="n">
+      <c r="D63" s="218" t="n">
         <v>44424</v>
       </c>
-      <c r="E63" s="2"/>
-      <c r="F63" s="2"/>
-      <c r="G63" s="2"/>
-      <c r="H63" s="170" t="s">
+      <c r="E63" s="216"/>
+      <c r="F63" s="216"/>
+      <c r="G63" s="216"/>
+      <c r="H63" s="219" t="s">
         <v>183</v>
       </c>
-      <c r="I63" s="4" t="n">
+      <c r="I63" s="218" t="n">
         <v>44425</v>
       </c>
-      <c r="J63" s="7">
+      <c r="J63" s="220">
         <f>I63-D63</f>
         <v>1</v>
       </c>
-      <c r="K63" s="171" t="s">
+      <c r="K63" s="221" t="s">
         <v>184</v>
       </c>
-      <c r="L63" s="4" t="n">
+      <c r="L63" s="218" t="n">
         <v>44425</v>
       </c>
-      <c r="M63" s="2">
+      <c r="M63" s="216">
         <f>L63-D63</f>
         <v>1</v>
       </c>
-      <c r="N63" s="2"/>
-      <c r="O63" s="2"/>
-      <c r="P63" s="2"/>
+      <c r="N63" s="216"/>
+      <c r="O63" s="216"/>
+      <c r="P63" s="216"/>
+    </row>
+    <row r="64" spans="1:16">
+      <c r="A64" s="184" t="s">
+        <v>10</v>
+      </c>
+      <c r="B64" s="184" t="s">
+        <v>11</v>
+      </c>
+      <c r="C64" s="185" t="s">
+        <v>185</v>
+      </c>
+      <c r="D64" s="186" t="n">
+        <v>44432</v>
+      </c>
+      <c r="E64" s="184"/>
+      <c r="F64" s="184"/>
+      <c r="G64" s="184"/>
+      <c r="H64" s="187" t="s">
+        <v>186</v>
+      </c>
+      <c r="I64" s="186" t="n">
+        <v>44432</v>
+      </c>
+      <c r="J64" s="7">
+        <f>I64-D64</f>
+        <v>0</v>
+      </c>
+      <c r="K64" s="188" t="s">
+        <v>187</v>
+      </c>
+      <c r="L64" s="189" t="n">
+        <v>44432</v>
+      </c>
+      <c r="M64" s="2">
+        <f>L64-D64</f>
+        <v>0</v>
+      </c>
+      <c r="N64" s="184"/>
+      <c r="O64" s="184"/>
+      <c r="P64" s="184"/>
+    </row>
+    <row r="65" spans="1:16">
+      <c r="A65" s="184" t="s">
+        <v>10</v>
+      </c>
+      <c r="B65" s="184" t="s">
+        <v>11</v>
+      </c>
+      <c r="C65" s="190" t="s">
+        <v>188</v>
+      </c>
+      <c r="D65" s="186" t="n">
+        <v>44446</v>
+      </c>
+      <c r="E65" s="184"/>
+      <c r="F65" s="184"/>
+      <c r="G65" s="184"/>
+      <c r="H65" s="184"/>
+      <c r="I65" s="184"/>
+      <c r="J65" s="184"/>
+      <c r="K65" s="184"/>
+      <c r="L65" s="184"/>
+      <c r="M65" s="184"/>
+      <c r="N65" s="184"/>
+      <c r="O65" s="184"/>
+      <c r="P65" s="184"/>
+    </row>
+    <row r="66" spans="1:16">
+      <c r="A66" s="184" t="s">
+        <v>10</v>
+      </c>
+      <c r="B66" s="184" t="s">
+        <v>11</v>
+      </c>
+      <c r="C66" s="191" t="s">
+        <v>189</v>
+      </c>
+      <c r="D66" s="186" t="n">
+        <v>44446</v>
+      </c>
+      <c r="E66" s="184"/>
+      <c r="F66" s="184"/>
+      <c r="G66" s="184"/>
+      <c r="H66" s="192" t="s">
+        <v>190</v>
+      </c>
+      <c r="I66" s="189" t="n">
+        <v>44448</v>
+      </c>
+      <c r="J66" s="7">
+        <f>I66-D66</f>
+        <v>2</v>
+      </c>
+      <c r="K66" s="193" t="s">
+        <v>191</v>
+      </c>
+      <c r="L66" s="189" t="n">
+        <v>44447</v>
+      </c>
+      <c r="M66" s="2">
+        <f>L66-D66</f>
+        <v>1</v>
+      </c>
+      <c r="N66" s="184"/>
+      <c r="O66" s="184"/>
+      <c r="P66" s="184"/>
+    </row>
+    <row r="67" spans="1:16">
+      <c r="A67" s="184" t="s">
+        <v>10</v>
+      </c>
+      <c r="B67" s="184" t="s">
+        <v>11</v>
+      </c>
+      <c r="C67" s="194" t="s">
+        <v>192</v>
+      </c>
+      <c r="D67" s="186" t="n">
+        <v>44452</v>
+      </c>
+      <c r="E67" s="184"/>
+      <c r="F67" s="184"/>
+      <c r="G67" s="184"/>
+      <c r="H67" s="184"/>
+      <c r="I67" s="184"/>
+      <c r="J67" s="184"/>
+      <c r="K67" s="195" t="s">
+        <v>193</v>
+      </c>
+      <c r="L67" s="189" t="n">
+        <v>44453</v>
+      </c>
+      <c r="M67" s="2">
+        <f>L67-D67</f>
+        <v>1</v>
+      </c>
+      <c r="N67" s="184"/>
+      <c r="O67" s="184"/>
+      <c r="P67" s="184"/>
+    </row>
+    <row r="68" spans="1:16">
+      <c r="A68" s="184" t="s">
+        <v>10</v>
+      </c>
+      <c r="B68" s="184" t="s">
+        <v>11</v>
+      </c>
+      <c r="C68" s="196" t="s">
+        <v>194</v>
+      </c>
+      <c r="D68" s="186" t="n">
+        <v>44452</v>
+      </c>
+      <c r="E68" s="184"/>
+      <c r="F68" s="184"/>
+      <c r="G68" s="184"/>
+      <c r="H68" s="184"/>
+      <c r="I68" s="184"/>
+      <c r="J68" s="184"/>
+      <c r="K68" s="197" t="s">
+        <v>195</v>
+      </c>
+      <c r="L68" s="189" t="n">
+        <v>44454</v>
+      </c>
+      <c r="M68" s="2">
+        <f>L68-D68</f>
+        <v>2</v>
+      </c>
+      <c r="N68" s="184"/>
+      <c r="O68" s="184"/>
+      <c r="P68" s="184"/>
+    </row>
+    <row r="69" spans="1:16">
+      <c r="A69" s="184" t="s">
+        <v>10</v>
+      </c>
+      <c r="B69" s="184" t="s">
+        <v>11</v>
+      </c>
+      <c r="C69" s="198" t="s">
+        <v>196</v>
+      </c>
+      <c r="D69" s="186" t="n">
+        <v>44452</v>
+      </c>
+      <c r="E69" s="184"/>
+      <c r="F69" s="184"/>
+      <c r="G69" s="184"/>
+      <c r="H69" s="184"/>
+      <c r="I69" s="184"/>
+      <c r="J69" s="184"/>
+      <c r="K69" s="199" t="s">
+        <v>197</v>
+      </c>
+      <c r="L69" s="186" t="n">
+        <v>44454</v>
+      </c>
+      <c r="M69" s="2">
+        <f>L69-D69</f>
+        <v>2</v>
+      </c>
+      <c r="N69" s="184"/>
+      <c r="O69" s="184"/>
+      <c r="P69" s="184"/>
+    </row>
+    <row r="70" spans="1:16">
+      <c r="A70" s="184" t="s">
+        <v>10</v>
+      </c>
+      <c r="B70" s="184" t="s">
+        <v>76</v>
+      </c>
+      <c r="C70" s="200" t="s">
+        <v>198</v>
+      </c>
+      <c r="D70" s="186" t="n">
+        <v>44454</v>
+      </c>
+      <c r="E70" s="184"/>
+      <c r="F70" s="184"/>
+      <c r="G70" s="184"/>
+      <c r="H70" s="184"/>
+      <c r="I70" s="184"/>
+      <c r="J70" s="184"/>
+      <c r="K70" s="201" t="s">
+        <v>199</v>
+      </c>
+      <c r="L70" s="189" t="n">
+        <v>44455</v>
+      </c>
+      <c r="M70" s="2">
+        <f>L70-D70</f>
+        <v>1</v>
+      </c>
+      <c r="N70" s="184"/>
+      <c r="O70" s="184"/>
+      <c r="P70" s="184"/>
+    </row>
+    <row r="71" spans="1:16">
+      <c r="A71" s="184" t="s">
+        <v>10</v>
+      </c>
+      <c r="B71" s="184" t="s">
+        <v>76</v>
+      </c>
+      <c r="C71" s="202" t="s">
+        <v>200</v>
+      </c>
+      <c r="D71" s="186" t="n">
+        <v>44460</v>
+      </c>
+      <c r="E71" s="184"/>
+      <c r="F71" s="184"/>
+      <c r="G71" s="184"/>
+      <c r="H71" s="184"/>
+      <c r="I71" s="184"/>
+      <c r="J71" s="184"/>
+      <c r="K71" s="203" t="s">
+        <v>201</v>
+      </c>
+      <c r="L71" s="189" t="n">
+        <v>44462</v>
+      </c>
+      <c r="M71" s="2">
+        <f>L71-D71</f>
+        <v>2</v>
+      </c>
+      <c r="N71" s="184"/>
+      <c r="O71" s="184"/>
+      <c r="P71" s="184"/>
+    </row>
+    <row r="72" spans="1:16">
+      <c r="A72" s="184" t="s">
+        <v>10</v>
+      </c>
+      <c r="B72" s="184" t="s">
+        <v>76</v>
+      </c>
+      <c r="C72" s="204" t="s">
+        <v>202</v>
+      </c>
+      <c r="D72" s="186" t="n">
+        <v>44460</v>
+      </c>
+      <c r="E72" s="184"/>
+      <c r="F72" s="184"/>
+      <c r="G72" s="184"/>
+      <c r="H72" s="184"/>
+      <c r="I72" s="184"/>
+      <c r="J72" s="184"/>
+      <c r="K72" s="205" t="s">
+        <v>203</v>
+      </c>
+      <c r="L72" s="189" t="n">
+        <v>44462</v>
+      </c>
+      <c r="M72" s="2">
+        <f>L72-D72</f>
+        <v>2</v>
+      </c>
+      <c r="N72" s="184"/>
+      <c r="O72" s="184"/>
+      <c r="P72" s="184"/>
+    </row>
+    <row r="73" spans="1:16">
+      <c r="A73" s="184" t="s">
+        <v>10</v>
+      </c>
+      <c r="B73" s="184" t="s">
+        <v>76</v>
+      </c>
+      <c r="C73" s="206" t="s">
+        <v>204</v>
+      </c>
+      <c r="D73" s="186" t="n">
+        <v>44460</v>
+      </c>
+      <c r="E73" s="184"/>
+      <c r="F73" s="184"/>
+      <c r="G73" s="184"/>
+      <c r="H73" s="184"/>
+      <c r="I73" s="184"/>
+      <c r="J73" s="184"/>
+      <c r="K73" s="207" t="s">
+        <v>205</v>
+      </c>
+      <c r="L73" s="189" t="n">
+        <v>44462</v>
+      </c>
+      <c r="M73" s="2">
+        <f>L73-D73</f>
+        <v>2</v>
+      </c>
+      <c r="N73" s="184"/>
+      <c r="O73" s="184"/>
+      <c r="P73" s="184"/>
+    </row>
+    <row r="74" spans="1:16">
+      <c r="A74" s="184" t="s">
+        <v>10</v>
+      </c>
+      <c r="B74" s="184" t="s">
+        <v>76</v>
+      </c>
+      <c r="C74" s="208" t="s">
+        <v>206</v>
+      </c>
+      <c r="D74" s="186" t="n">
+        <v>44460</v>
+      </c>
+      <c r="E74" s="184"/>
+      <c r="F74" s="184"/>
+      <c r="G74" s="184"/>
+      <c r="H74" s="184"/>
+      <c r="I74" s="184"/>
+      <c r="J74" s="184"/>
+      <c r="K74" s="209" t="s">
+        <v>207</v>
+      </c>
+      <c r="L74" s="189" t="n">
+        <v>44464</v>
+      </c>
+      <c r="M74" s="2">
+        <f>L74-D74</f>
+        <v>4</v>
+      </c>
+      <c r="N74" s="184"/>
+      <c r="O74" s="184"/>
+      <c r="P74" s="184"/>
+    </row>
+    <row r="75" spans="1:16">
+      <c r="A75" s="184" t="s">
+        <v>10</v>
+      </c>
+      <c r="B75" s="184" t="s">
+        <v>76</v>
+      </c>
+      <c r="C75" s="210" t="s">
+        <v>208</v>
+      </c>
+      <c r="D75" s="186" t="n">
+        <v>44460</v>
+      </c>
+      <c r="E75" s="184"/>
+      <c r="F75" s="184"/>
+      <c r="G75" s="184"/>
+      <c r="H75" s="184"/>
+      <c r="I75" s="184"/>
+      <c r="J75" s="184"/>
+      <c r="K75" s="211" t="s">
+        <v>209</v>
+      </c>
+      <c r="L75" s="186" t="n">
+        <v>44464</v>
+      </c>
+      <c r="M75" s="2">
+        <f>L75-D75</f>
+        <v>4</v>
+      </c>
+      <c r="N75" s="184"/>
+      <c r="O75" s="184"/>
+      <c r="P75" s="184"/>
+    </row>
+    <row r="76" spans="1:16">
+      <c r="A76" s="184" t="s">
+        <v>10</v>
+      </c>
+      <c r="B76" s="184" t="s">
+        <v>11</v>
+      </c>
+      <c r="C76" s="212" t="s">
+        <v>210</v>
+      </c>
+      <c r="D76" s="186" t="n">
+        <v>44460</v>
+      </c>
+      <c r="E76" s="184"/>
+      <c r="F76" s="184"/>
+      <c r="G76" s="184"/>
+      <c r="H76" s="184"/>
+      <c r="I76" s="184"/>
+      <c r="J76" s="184"/>
+      <c r="K76" s="213" t="s">
+        <v>211</v>
+      </c>
+      <c r="L76" s="186" t="n">
+        <v>44464</v>
+      </c>
+      <c r="M76" s="2">
+        <f>L76-D76</f>
+        <v>4</v>
+      </c>
+      <c r="N76" s="184"/>
+      <c r="O76" s="184"/>
+      <c r="P76" s="184"/>
+    </row>
+    <row r="77" spans="1:16">
+      <c r="A77" s="184" t="s">
+        <v>10</v>
+      </c>
+      <c r="B77" s="184" t="s">
+        <v>11</v>
+      </c>
+      <c r="C77" s="214" t="s">
+        <v>212</v>
+      </c>
+      <c r="D77" s="186" t="n">
+        <v>44466</v>
+      </c>
+      <c r="E77" s="184"/>
+      <c r="F77" s="184"/>
+      <c r="G77" s="184"/>
+      <c r="H77" s="184"/>
+      <c r="I77" s="184"/>
+      <c r="J77" s="184"/>
+      <c r="K77" s="215" t="s">
+        <v>213</v>
+      </c>
+      <c r="L77" s="189" t="n">
+        <v>44466</v>
+      </c>
+      <c r="M77" s="2">
+        <f>L77-D77</f>
+        <v>0</v>
+      </c>
+      <c r="N77" s="184"/>
+      <c r="O77" s="184"/>
+      <c r="P77" s="184"/>
+    </row>
+    <row r="78" spans="4:4">
+      <c r="D78" s="180"/>
+    </row>
+    <row r="93" spans="4:4">
+      <c r="D93" s="180"/>
+    </row>
+    <row r="94" spans="4:4">
+      <c r="D94" s="181"/>
+    </row>
+    <row r="95" spans="4:4">
+      <c r="D95" s="182"/>
+    </row>
+    <row r="96" spans="4:4">
+      <c r="D96" s="180"/>
+    </row>
+    <row r="97" spans="4:4">
+      <c r="D97" s="180"/>
+    </row>
+    <row r="98" spans="4:4">
+      <c r="D98" s="180"/>
+    </row>
+    <row r="99" spans="4:4">
+      <c r="D99" s="180"/>
+    </row>
+    <row r="100" spans="4:4">
+      <c r="D100" s="180"/>
+    </row>
+    <row r="101" spans="4:4">
+      <c r="D101" s="180"/>
+    </row>
+    <row r="102" spans="4:4">
+      <c r="D102" s="180"/>
+    </row>
+    <row r="103" spans="4:4">
+      <c r="D103" s="180"/>
+    </row>
+    <row r="104" spans="4:4">
+      <c r="D104" s="180"/>
+    </row>
+    <row r="105" spans="4:4">
+      <c r="D105" s="180"/>
+    </row>
+    <row r="106" spans="4:4">
+      <c r="D106" s="180"/>
+    </row>
+    <row r="107" spans="4:4">
+      <c r="D107" s="180"/>
+    </row>
+    <row r="108" spans="4:4">
+      <c r="D108" s="183"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -7844,11 +9174,40 @@
     <hyperlink ref="C63" r:id="rId163"/>
     <hyperlink ref="H63" r:id="rId164"/>
     <hyperlink ref="K63" r:id="rId165"/>
+    <hyperlink ref="C64" r:id="rId166"/>
+    <hyperlink ref="H64" r:id="rId167"/>
+    <hyperlink ref="K64" r:id="rId168"/>
+    <hyperlink ref="C65" r:id="rId169"/>
+    <hyperlink ref="C66" r:id="rId170"/>
+    <hyperlink ref="H66" r:id="rId171"/>
+    <hyperlink ref="K66" r:id="rId172"/>
+    <hyperlink ref="C67" r:id="rId173"/>
+    <hyperlink ref="K67" r:id="rId174"/>
+    <hyperlink ref="C68" r:id="rId175"/>
+    <hyperlink ref="K68" r:id="rId176"/>
+    <hyperlink ref="C69" r:id="rId177"/>
+    <hyperlink ref="K69" r:id="rId178"/>
+    <hyperlink ref="C70" r:id="rId179"/>
+    <hyperlink ref="K70" r:id="rId180"/>
+    <hyperlink ref="C71" r:id="rId181"/>
+    <hyperlink ref="K71" r:id="rId182"/>
+    <hyperlink ref="C72" r:id="rId183"/>
+    <hyperlink ref="K72" r:id="rId184"/>
+    <hyperlink ref="C73" r:id="rId185"/>
+    <hyperlink ref="K73" r:id="rId186"/>
+    <hyperlink ref="C74" r:id="rId187"/>
+    <hyperlink ref="K74" r:id="rId188"/>
+    <hyperlink ref="C75" r:id="rId189"/>
+    <hyperlink ref="K75" r:id="rId190"/>
+    <hyperlink ref="C76" r:id="rId191"/>
+    <hyperlink ref="K76" r:id="rId192"/>
+    <hyperlink ref="C77" r:id="rId193"/>
+    <hyperlink ref="K77" r:id="rId194"/>
   </hyperlinks>
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1629269222" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1632926886" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -7857,15 +9216,15 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1629269222" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1629269222" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1632926886" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1632926886" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
-  <drawing r:id="rId166"/>
+  <drawing r:id="rId195"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1629269222" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1632926886" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>